<commit_message>
fixed state name columns
</commit_message>
<xml_diff>
--- a/Raw Data/Data Keys.xlsx
+++ b/Raw Data/Data Keys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96cc1363e59f2cdc/Data_Analysis_bootcamp/Module_20/dexter_project/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/96cc1363e59f2cdc/Data_Analysis_bootcamp/Module_20/dexter_project/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{B25D863A-E1C5-4A18-8E96-6A2D4B978B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99CEE470-7D16-46D3-ADA6-221FCA14C8F8}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{B25D863A-E1C5-4A18-8E96-6A2D4B978B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3468584F-CB9A-4412-AD31-41FF04C91584}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{C6FDEC38-CE45-4E93-A3E2-8C523C682540}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{C6FDEC38-CE45-4E93-A3E2-8C523C682540}"/>
   </bookViews>
   <sheets>
     <sheet name="weather data key" sheetId="1" r:id="rId1"/>
@@ -11227,7 +11227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EDD197-06E1-4BB9-A4F5-6F0F35893D58}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -25374,11 +25374,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BBA3FF-1263-48C1-9C7E-87F833A6D24C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>